<commit_message>
changes in xlsx file
</commit_message>
<xml_diff>
--- a/Parameters_for_diagnosis.xlsx
+++ b/Parameters_for_diagnosis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Faults in various sources" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="151">
   <si>
     <t>Compression fault</t>
   </si>
@@ -256,9 +256,6 @@
     <t>Lubrication System</t>
   </si>
   <si>
-    <t>Some parameters can be associated with more than 1 components, diagnostic combination of 2 methods (component and overall)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Exhaust gas boiler fouling/ blocked turbine exhaust </t>
   </si>
   <si>
@@ -455,13 +452,40 @@
   </si>
   <si>
     <t>Leaking exhaust valves</t>
+  </si>
+  <si>
+    <t>Air Filter</t>
+  </si>
+  <si>
+    <t>Some parameters can be associated with more than 1 component, diagnostic combination of 2 methods (component and overall)</t>
+  </si>
+  <si>
+    <t>Temperature Air Cooler IN (Air)</t>
+  </si>
+  <si>
+    <t>Temperature Air Cooler IN (Water)</t>
+  </si>
+  <si>
+    <t>Temperature Air Cooler Out (Air)</t>
+  </si>
+  <si>
+    <t>Temperature Air Cooler Out (Water)</t>
+  </si>
+  <si>
+    <t>From 1,2,3 the effectiveness can be calculated</t>
+  </si>
+  <si>
+    <t>If effectiveness is low</t>
+  </si>
+  <si>
+    <t>temperature water out</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -488,6 +512,22 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -525,12 +565,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -813,14 +860,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="52.7109375" customWidth="1"/>
-    <col min="3" max="3" width="64.42578125" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" customWidth="1"/>
+    <col min="3" max="3" width="50.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.7109375" customWidth="1"/>
     <col min="6" max="6" width="27.42578125" customWidth="1"/>
@@ -838,13 +886,13 @@
         <v>17</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -858,13 +906,13 @@
         <v>12</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -878,13 +926,13 @@
         <v>13</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -898,13 +946,13 @@
         <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -918,13 +966,13 @@
         <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -938,13 +986,13 @@
         <v>22</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -958,10 +1006,10 @@
         <v>23</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -975,10 +1023,10 @@
         <v>24</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -992,7 +1040,7 @@
         <v>25</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1014,7 +1062,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1025,7 +1073,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1033,7 +1081,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1041,7 +1089,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1049,7 +1097,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1057,47 +1105,47 @@
         <v>15</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C17" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C18" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C19" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C20" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C21" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C22" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C23" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C24" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
@@ -1106,7 +1154,7 @@
         <v>18</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1114,7 +1162,7 @@
         <v>19</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1122,7 +1170,7 @@
         <v>20</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1130,41 +1178,41 @@
         <v>21</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:1" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:1" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:1" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
@@ -1214,7 +1262,7 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection sqref="A1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,13 +1288,13 @@
         <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F2" t="s">
         <v>54</v>
       </c>
       <c r="G2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1257,13 +1305,13 @@
         <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F3" t="s">
         <v>55</v>
       </c>
       <c r="G3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1274,13 +1322,13 @@
         <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F4" t="s">
         <v>56</v>
       </c>
       <c r="G4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1291,13 +1339,13 @@
         <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F5" t="s">
         <v>57</v>
       </c>
       <c r="G5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1308,13 +1356,13 @@
         <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F6" t="s">
         <v>58</v>
       </c>
       <c r="G6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1325,13 +1373,13 @@
         <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G7" t="s">
         <v>93</v>
-      </c>
-      <c r="G7" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1342,13 +1390,13 @@
         <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F8" t="s">
         <v>65</v>
       </c>
       <c r="G8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1359,13 +1407,13 @@
         <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F9" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" t="s">
         <v>90</v>
-      </c>
-      <c r="G9" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1496,7 +1544,7 @@
         <v>50</v>
       </c>
       <c r="F22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1595,10 +1643,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1606,104 +1654,141 @@
     <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.28515625" customWidth="1"/>
     <col min="4" max="4" width="32.140625" customWidth="1"/>
-    <col min="5" max="5" width="30" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.28515625" customWidth="1"/>
     <col min="7" max="7" width="26.140625" customWidth="1"/>
     <col min="8" max="8" width="25.7109375" customWidth="1"/>
+    <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:9" s="5" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+      <c r="B1" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="C1" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Input data check for sensor errors
Created from Panos
</commit_message>
<xml_diff>
--- a/Parameters_for_diagnosis.xlsx
+++ b/Parameters_for_diagnosis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Faults in various sources" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="160">
   <si>
     <t>Compression fault</t>
   </si>
@@ -479,6 +479,33 @@
   </si>
   <si>
     <t>temperature water out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameters that have to be check before HC </t>
+  </si>
+  <si>
+    <t>Parameters that have to be checked after HC</t>
+  </si>
+  <si>
+    <t>AF pressure drop</t>
+  </si>
+  <si>
+    <t>Pscav - Pexh</t>
+  </si>
+  <si>
+    <t>FPI vs Power</t>
+  </si>
+  <si>
+    <t>Parameters that should be compared in absolut numbers and not in percentage</t>
+  </si>
+  <si>
+    <t>Texh</t>
+  </si>
+  <si>
+    <t>Energy equilibrium on TC shaft (C - T)</t>
+  </si>
+  <si>
+    <t>usually corrected to ISO using Tamb and TcwIN</t>
   </si>
 </sst>
 </file>
@@ -1259,28 +1286,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:O1048576"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="36.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="53.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.5703125" customWidth="1"/>
+    <col min="17" max="17" width="46" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="Q1" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1296,8 +1330,11 @@
       <c r="G2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="Q2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1313,8 +1350,11 @@
       <c r="G3" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="Q3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1330,8 +1370,11 @@
       <c r="G4" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="Q4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1347,8 +1390,11 @@
       <c r="G5" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="Q5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1365,7 +1411,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1382,7 +1428,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1399,7 +1445,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1416,12 +1462,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1429,7 +1475,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1437,7 +1483,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1445,7 +1491,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1455,8 +1501,11 @@
       <c r="F14" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="Q14" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1466,8 +1515,14 @@
       <c r="F15" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="Q15" t="s">
+        <v>36</v>
+      </c>
+      <c r="R15" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1477,8 +1532,14 @@
       <c r="F16" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="Q16" t="s">
+        <v>37</v>
+      </c>
+      <c r="R16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1488,8 +1549,14 @@
       <c r="F17" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="Q17" t="s">
+        <v>157</v>
+      </c>
+      <c r="R17" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1499,8 +1566,14 @@
       <c r="F18" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="Q18" t="s">
+        <v>38</v>
+      </c>
+      <c r="R18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1511,7 +1584,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1522,7 +1595,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1536,7 +1609,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1547,7 +1620,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1555,7 +1628,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1563,7 +1636,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1571,37 +1644,43 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F28" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1645,7 +1724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1654,7 +1733,7 @@
     <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.28515625" customWidth="1"/>
     <col min="4" max="4" width="32.140625" customWidth="1"/>
-    <col min="5" max="5" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.5703125" customWidth="1"/>
     <col min="6" max="6" width="27.28515625" customWidth="1"/>
     <col min="7" max="7" width="26.140625" customWidth="1"/>
     <col min="8" max="8" width="25.7109375" customWidth="1"/>

</xml_diff>